<commit_message>
Update: add test case
</commit_message>
<xml_diff>
--- a/設計/フロントエンドテスト仕様書.xlsx
+++ b/設計/フロントエンドテスト仕様書.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\rework\smoking-area-count\設計\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\smoking-area-count\設計\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D79CA1-6A65-4461-8AF7-40963D648B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FE74B-F343-4C55-B248-F707DF3177CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="900" windowWidth="21600" windowHeight="15735" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30990" yWindow="3645" windowWidth="21600" windowHeight="12735" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="テスト仕様書" sheetId="3" r:id="rId1"/>
@@ -21,27 +21,27 @@
   </externalReferences>
   <definedNames>
     <definedName name="[開本]工程分類">[1]開本変換表!$B$5:$B$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">テスト仕様書!$2:$2</definedName>
     <definedName name="T_ComChkEnm">#REF!</definedName>
     <definedName name="TL1_Command_Mode">#REF!</definedName>
-    <definedName name="Z_07C937DF_9B19_4F7A_953B_7CA7C53509E7_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_1222CA57_929A_41D4_BE25_9E592A6AB8DE_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_35186B6A_34F9_409B_B314_085999155EE0_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_571D7DD0_C3F2_4400_8F70_D9DE1CA826B4_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_8940A7A4_D80A_41E7_90B2_B7572E6D6A8B_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
+    <definedName name="Z_07C937DF_9B19_4F7A_953B_7CA7C53509E7_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_1222CA57_929A_41D4_BE25_9E592A6AB8DE_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_35186B6A_34F9_409B_B314_085999155EE0_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_571D7DD0_C3F2_4400_8F70_D9DE1CA826B4_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_8940A7A4_D80A_41E7_90B2_B7572E6D6A8B_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
     <definedName name="Z_8940A7A4_D80A_41E7_90B2_B7572E6D6A8B_.wvu.PrintTitles" localSheetId="0" hidden="1">テスト仕様書!$2:$2</definedName>
     <definedName name="Z_90CA437D_40FA_44A6_913A_9B189FB4FA56_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$2</definedName>
-    <definedName name="Z_9A4A52C3_004B_4B00_AB06_BD7C0B37F0A9_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
+    <definedName name="Z_9A4A52C3_004B_4B00_AB06_BD7C0B37F0A9_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
     <definedName name="Z_9A4A52C3_004B_4B00_AB06_BD7C0B37F0A9_.wvu.PrintTitles" localSheetId="0" hidden="1">テスト仕様書!$2:$2</definedName>
-    <definedName name="Z_AF32C4FA_C889_45CE_9C32_0FFDDAAC9065_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_B06E16AB_6449_4306_BA78_66DC7F0824D7_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_B136BE0D_E2CA_4C2F_8BDD_76669C95D83A_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
+    <definedName name="Z_AF32C4FA_C889_45CE_9C32_0FFDDAAC9065_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_B06E16AB_6449_4306_BA78_66DC7F0824D7_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_B136BE0D_E2CA_4C2F_8BDD_76669C95D83A_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
     <definedName name="Z_B136BE0D_E2CA_4C2F_8BDD_76669C95D83A_.wvu.PrintTitles" localSheetId="0" hidden="1">テスト仕様書!$2:$2</definedName>
-    <definedName name="Z_E7B8B120_CB48_4066_9DB6_4F9FA0ABCF37_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_EB73383E_98D3_4306_B074_8992ED4F2B32_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_ED114405_3395_4F36_905B_4A2A230A5603_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
-    <definedName name="Z_F67BDF4A_ADEB_46A9_9C1D_3656A2B8502F_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$340</definedName>
+    <definedName name="Z_E7B8B120_CB48_4066_9DB6_4F9FA0ABCF37_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_EB73383E_98D3_4306_B074_8992ED4F2B32_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_ED114405_3395_4F36_905B_4A2A230A5603_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
+    <definedName name="Z_F67BDF4A_ADEB_46A9_9C1D_3656A2B8502F_.wvu.FilterData" localSheetId="0" hidden="1">テスト仕様書!$B$2:$F$341</definedName>
     <definedName name="Z_F67BDF4A_ADEB_46A9_9C1D_3656A2B8502F_.wvu.PrintTitles" localSheetId="0" hidden="1">テスト仕様書!$2:$2</definedName>
     <definedName name="インターフェース">[2]参考資料!#REF!</definedName>
     <definedName name="キャスト">[2]参考資料!#REF!</definedName>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>項番</t>
   </si>
@@ -1033,28 +1033,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>CSVに一行手動で加え、更新されるかを目視で確認</t>
-    <rPh sb="4" eb="6">
-      <t>イチギョウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シュドウ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>クワ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>モクシ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>設定ファイルに存在しないCSVファイルを設定した際に画面には0人と表示されること</t>
     <rPh sb="0" eb="2">
       <t>セッテイ</t>
@@ -1181,6 +1159,95 @@
     </rPh>
     <rPh sb="43" eb="45">
       <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>タイトルに「喫煙室利用者数カウント」と表示されていること</t>
+    <rPh sb="19" eb="21">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>タブバーに「喫煙室利用者数カウント」と表示されていること</t>
+    <rPh sb="19" eb="21">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ログファイルを編集しカードの色が変更されることを目視で確認</t>
+    <rPh sb="7" eb="9">
+      <t>ヘンシュウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>イロ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>モクシ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>画像表示中に利用者が定員上限以上になった場合、アラート部の色が変更されること</t>
+    <rPh sb="0" eb="2">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>ヒョウジチュウ</t>
+    </rPh>
+    <rPh sb="6" eb="9">
+      <t>リヨウシャ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>テイイン</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ブ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>イロ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CSVに手動で一行追加し、更新されるかを目視で確認</t>
+    <rPh sb="4" eb="6">
+      <t>シュドウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イチギョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>モクシ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -1963,6 +2030,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1983,9 +2053,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2480,13 +2547,13 @@
     <tabColor theme="5" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G346"/>
+  <dimension ref="A1:G347"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2504,8 +2571,8 @@
     <row r="1" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B1" s="18"/>
       <c r="C1" s="1">
-        <f>SUBTOTAL(3,C3:C335)</f>
-        <v>28</v>
+        <f>SUBTOTAL(3,C3:C336)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -2534,7 +2601,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>35</v>
@@ -2551,7 +2618,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>35</v>
@@ -2561,14 +2628,14 @@
     </row>
     <row r="5" spans="2:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B5" s="2">
-        <f t="shared" ref="B5:B68" si="0">B4+1</f>
+        <f t="shared" ref="B5:B69" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>35</v>
@@ -2585,7 +2652,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>35</v>
@@ -2599,10 +2666,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>35</v>
@@ -2695,29 +2762,31 @@
       <c r="F12" s="3"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:7" ht="27" x14ac:dyDescent="0.15">
       <c r="B13" s="2">
-        <f t="shared" si="0"/>
+        <f>B12+1</f>
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E13" s="21"/>
       <c r="F13" s="3"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="2:7" ht="54" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:7" ht="27" x14ac:dyDescent="0.15">
       <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>35</v>
@@ -2725,16 +2794,16 @@
       <c r="F14" s="3"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:7" ht="54" x14ac:dyDescent="0.15">
       <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>26</v>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>35</v>
@@ -2742,16 +2811,16 @@
       <c r="F15" s="3"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="2:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>35</v>
@@ -2759,16 +2828,16 @@
       <c r="F16" s="3"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="27" x14ac:dyDescent="0.15">
       <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
+      <c r="C17" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>35</v>
@@ -2782,7 +2851,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>34</v>
@@ -2798,8 +2867,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>17</v>
+      <c r="C19" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>34</v>
@@ -2815,8 +2884,8 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>20</v>
+      <c r="C20" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>34</v>
@@ -2833,7 +2902,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>34</v>
@@ -2850,7 +2919,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>34</v>
@@ -2861,32 +2930,30 @@
       <c r="F22" s="3"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="2:7" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B23" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>22</v>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>32</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>38</v>
@@ -2894,50 +2961,50 @@
       <c r="E24" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="2:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B25" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="2:7" ht="81" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="27" x14ac:dyDescent="0.15">
       <c r="B26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>24</v>
+      <c r="C26" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>33</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="81" x14ac:dyDescent="0.15">
       <c r="B27" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>38</v>
@@ -2945,19 +3012,21 @@
       <c r="E27" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="2:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>35</v>
@@ -2971,10 +3040,10 @@
         <v>27</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>35</v>
@@ -2988,10 +3057,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>51</v>
+        <v>31</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>35</v>
@@ -2999,14 +3068,20 @@
       <c r="F30" s="3"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:7" ht="27" x14ac:dyDescent="0.15">
       <c r="B31" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="21"/>
+      <c r="C31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="14"/>
     </row>
@@ -3015,9 +3090,15 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="21"/>
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="14"/>
     </row>
@@ -3026,9 +3107,15 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="21"/>
+      <c r="C33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="14"/>
     </row>
@@ -3419,7 +3506,7 @@
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B69" s="2">
-        <f t="shared" ref="B69:B132" si="1">B68+1</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="C69" s="3"/>
@@ -3430,7 +3517,7 @@
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B70" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B70:B133" si="1">B69+1</f>
         <v>68</v>
       </c>
       <c r="C70" s="3"/>
@@ -4123,7 +4210,7 @@
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B133" s="2">
-        <f t="shared" ref="B133:B196" si="2">B132+1</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="C133" s="3"/>
@@ -4134,7 +4221,7 @@
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B134" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B134:B197" si="2">B133+1</f>
         <v>132</v>
       </c>
       <c r="C134" s="3"/>
@@ -4827,7 +4914,7 @@
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B197" s="2">
-        <f t="shared" ref="B197:B260" si="3">B196+1</f>
+        <f t="shared" si="2"/>
         <v>195</v>
       </c>
       <c r="C197" s="3"/>
@@ -4838,7 +4925,7 @@
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B198" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B198:B261" si="3">B197+1</f>
         <v>196</v>
       </c>
       <c r="C198" s="3"/>
@@ -5531,7 +5618,7 @@
     </row>
     <row r="261" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B261" s="2">
-        <f t="shared" ref="B261:B324" si="4">B260+1</f>
+        <f t="shared" si="3"/>
         <v>259</v>
       </c>
       <c r="C261" s="3"/>
@@ -5542,7 +5629,7 @@
     </row>
     <row r="262" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B262" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B262:B325" si="4">B261+1</f>
         <v>260</v>
       </c>
       <c r="C262" s="3"/>
@@ -6235,7 +6322,7 @@
     </row>
     <row r="325" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B325" s="2">
-        <f t="shared" ref="B325:B335" si="5">B324+1</f>
+        <f t="shared" si="4"/>
         <v>323</v>
       </c>
       <c r="C325" s="3"/>
@@ -6246,7 +6333,7 @@
     </row>
     <row r="326" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B326" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="B326:B336" si="5">B325+1</f>
         <v>324</v>
       </c>
       <c r="C326" s="3"/>
@@ -6343,8 +6430,8 @@
       <c r="F334" s="3"/>
       <c r="G334" s="14"/>
     </row>
-    <row r="335" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B335" s="4">
+    <row r="335" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B335" s="2">
         <f t="shared" si="5"/>
         <v>333</v>
       </c>
@@ -6354,65 +6441,67 @@
       <c r="F335" s="3"/>
       <c r="G335" s="14"/>
     </row>
-    <row r="336" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B336" s="23" t="s">
+    <row r="336" spans="2:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B336" s="4">
+        <f t="shared" si="5"/>
+        <v>334</v>
+      </c>
+      <c r="C336" s="3"/>
+      <c r="D336" s="3"/>
+      <c r="E336" s="21"/>
+      <c r="F336" s="3"/>
+      <c r="G336" s="14"/>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B337" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C336" s="24"/>
-      <c r="D336" s="24"/>
-      <c r="E336" s="24"/>
-      <c r="F336" s="25"/>
-      <c r="G336" s="12"/>
-    </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B337" s="26"/>
-      <c r="C337" s="24"/>
-      <c r="D337" s="24"/>
-      <c r="E337" s="24"/>
-      <c r="F337" s="25"/>
+      <c r="C337" s="25"/>
+      <c r="D337" s="25"/>
+      <c r="E337" s="25"/>
+      <c r="F337" s="26"/>
       <c r="G337" s="12"/>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B338" s="26"/>
-      <c r="C338" s="24"/>
-      <c r="D338" s="24"/>
-      <c r="E338" s="24"/>
-      <c r="F338" s="25"/>
+      <c r="B338" s="27"/>
+      <c r="C338" s="25"/>
+      <c r="D338" s="25"/>
+      <c r="E338" s="25"/>
+      <c r="F338" s="26"/>
       <c r="G338" s="12"/>
     </row>
-    <row r="339" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A339" s="5"/>
-      <c r="B339" s="26"/>
-      <c r="C339" s="24"/>
-      <c r="D339" s="24"/>
-      <c r="E339" s="24"/>
-      <c r="F339" s="25"/>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B339" s="27"/>
+      <c r="C339" s="25"/>
+      <c r="D339" s="25"/>
+      <c r="E339" s="25"/>
+      <c r="F339" s="26"/>
       <c r="G339" s="12"/>
     </row>
-    <row r="340" spans="1:7" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A340" s="5"/>
       <c r="B340" s="27"/>
-      <c r="C340" s="28"/>
-      <c r="D340" s="28"/>
-      <c r="E340" s="28"/>
-      <c r="F340" s="29"/>
+      <c r="C340" s="25"/>
+      <c r="D340" s="25"/>
+      <c r="E340" s="25"/>
+      <c r="F340" s="26"/>
       <c r="G340" s="12"/>
     </row>
-    <row r="341" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:7" s="8" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A341" s="5"/>
-      <c r="B341" s="19"/>
-      <c r="C341" s="6"/>
-      <c r="D341" s="6"/>
-      <c r="E341" s="13"/>
-      <c r="F341" s="5"/>
-      <c r="G341" s="5"/>
-    </row>
-    <row r="342" spans="1:7" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="B341" s="28"/>
+      <c r="C341" s="29"/>
+      <c r="D341" s="29"/>
+      <c r="E341" s="29"/>
+      <c r="F341" s="30"/>
+      <c r="G341" s="12"/>
+    </row>
+    <row r="342" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A342" s="5"/>
       <c r="B342" s="19"/>
-      <c r="C342" s="5"/>
-      <c r="D342" s="5"/>
-      <c r="E342" s="16"/>
+      <c r="C342" s="6"/>
+      <c r="D342" s="6"/>
+      <c r="E342" s="13"/>
       <c r="F342" s="5"/>
       <c r="G342" s="5"/>
     </row>
@@ -6425,11 +6514,14 @@
       <c r="F343" s="5"/>
       <c r="G343" s="5"/>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:7" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="A344" s="5"/>
       <c r="B344" s="19"/>
       <c r="C344" s="5"/>
       <c r="D344" s="5"/>
       <c r="E344" s="16"/>
+      <c r="F344" s="5"/>
+      <c r="G344" s="5"/>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B345" s="19"/>
@@ -6443,8 +6535,14 @@
       <c r="D346" s="5"/>
       <c r="E346" s="16"/>
     </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B347" s="19"/>
+      <c r="C347" s="5"/>
+      <c r="D347" s="5"/>
+      <c r="E347" s="16"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:F340" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="B2:F341" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <customSheetViews>
     <customSheetView guid="{B136BE0D-E2CA-4C2F-8BDD-76669C95D83A}" scale="80" fitToPage="1" showAutoFilter="1">
       <pane xSplit="3" ySplit="2" topLeftCell="F51" activePane="bottomRight" state="frozen"/>
@@ -6488,7 +6586,7 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
-    <mergeCell ref="B336:F340"/>
+    <mergeCell ref="B337:F341"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.59055118110236227" right="0.39370078740157483" top="0.59055118110236227" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>